<commit_message>
200321 (Back수정 완료, Excel 다운중)
</commit_message>
<xml_diff>
--- a/prepare_db/골든브릿지자산운용_김대중_펀드매니저 상세정보_운용펀드(기준일)_20200321.xlsx
+++ b/prepare_db/골든브릿지자산운용_김대중_펀드매니저 상세정보_운용펀드(기준일)_20200321.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,7 +533,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>골든브릿지스마트단기채증권투자신탁 1[채권]</t>
+          <t>대신공모주30증권자투자신탁 2[채권혼합](운용)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -544,52 +544,52 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2017-06-22</t>
+          <t>2016-01-11</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2018-08-27</t>
+          <t>2016-01-11</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">           1,219</t>
+          <t xml:space="preserve">             665</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve">           1,178</t>
+          <t xml:space="preserve">             692</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>채권형</t>
+          <t>혼합채권형</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>국내</t>
+          <t>혼합</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>0.14</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0.32</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>-2.60</t>
+          <t>13.15</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -609,19 +609,19 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0.07</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>┖▷골든브릿지스마트단기채증권투자신탁 1[채권]종류CF</t>
+          <t>┖▷대신공모주30증권자투자신탁 2[채권혼합]ClassA</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -632,27 +632,27 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2017-06-22</t>
+          <t>2016-01-15</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2018-08-27</t>
+          <t>2016-01-11</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t xml:space="preserve">             300</t>
+          <t xml:space="preserve">             208</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve">             285</t>
+          <t xml:space="preserve">             217</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>채권형</t>
+          <t>혼합채권형</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -662,54 +662,54 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>0.28</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>-4.99</t>
+          <t>8.92</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.89</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.89</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0.07</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>┖▷골든브릿지스마트단기채증권투자신탁 1[채권]종류CW</t>
+          <t>┖▷대신공모주30증권자투자신탁 2[채권혼합]ClassC</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -720,27 +720,27 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2017-06-22</t>
+          <t>2016-01-15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2018-08-27</t>
+          <t>2016-01-11</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t xml:space="preserve">             919</t>
+          <t xml:space="preserve">             457</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve">             893</t>
+          <t xml:space="preserve">             475</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>채권형</t>
+          <t>혼합채권형</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -750,27 +750,27 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>0.13</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>0.29</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>-2.83</t>
+          <t>7.56</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>1.19</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
@@ -780,12 +780,12 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>1.19</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0.07</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>골든브릿지으뜸단기증권투자신탁 1[채권]</t>
+          <t>대신배당공모주알파30증권투자신탁[채권혼합]운용</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -808,27 +808,27 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2017-10-20</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2018-08-27</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">             222</t>
+          <t xml:space="preserve">           5,830</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve">             220</t>
+          <t xml:space="preserve">           5,709</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>채권형</t>
+          <t>혼합채권형</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -838,22 +838,22 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>-1.91</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>0.17</t>
+          <t>-0.20</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>0.40</t>
+          <t>-1.27</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>0.11</t>
+          <t>7.58</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -873,7 +873,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0.07</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>┖▷골든브릿지으뜸단기증권투자신탁 1[채권]종류CF</t>
+          <t>┖▷대신배당공모주알파30증권투자신탁[채권혼합]Class A</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -896,27 +896,27 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2017-10-20</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2018-08-27</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">             201</t>
+          <t xml:space="preserve">              98</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t xml:space="preserve">             200</t>
+          <t xml:space="preserve">              97</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>채권형</t>
+          <t>혼합채권형</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -926,42 +926,42 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>-1.97</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>0.15</t>
+          <t>-0.54</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>0.36</t>
+          <t>-1.94</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>-0.07</t>
+          <t>4.72</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.69</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.50</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>0.04</t>
+          <t>0.69</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0.07</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>┖▷골든브릿지으뜸단기증권투자신탁 1[채권]종류CW</t>
+          <t>┖▷대신배당공모주알파30증권투자신탁[채권혼합]ClassC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -984,27 +984,27 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2017-10-20</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2018-08-27</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t xml:space="preserve">              20</t>
+          <t xml:space="preserve">           5,275</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t xml:space="preserve">              20</t>
+          <t xml:space="preserve">           5,164</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>채권형</t>
+          <t>혼합채권형</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1014,27 +1014,27 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.02</t>
+          <t>-1.99</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>0.16</t>
+          <t>-0.69</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>0.37</t>
+          <t>-2.24</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>-0.05</t>
+          <t>3.49</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>0.99</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1044,24 +1044,24 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>0.99</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0.07</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>골든브릿지베스트증권투자신탁 1[채권]</t>
+          <t>┖▷대신배당공모주알파30증권투자신탁[채권혼합]ClassC-E</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -1072,27 +1072,27 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2019-03-21</t>
+          <t>2019-09-30</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2019-09-27</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">          54,655</t>
+          <t xml:space="preserve">               0</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t xml:space="preserve">          56,232</t>
+          <t xml:space="preserve">               0</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>채권형</t>
+          <t>혼합채권형</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1102,12 +1102,12 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.40</t>
+          <t>-1.96</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>1.47</t>
+          <t>0.00</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1117,12 +1117,12 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>3.03</t>
+          <t>-1.54</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.68</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1132,24 +1132,24 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>0.01</t>
+          <t>0.68</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.03</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>┖▷골든브릿지베스트증권투자신탁 1[채권]종류C-F</t>
+          <t>┖▷대신배당공모주알파30증권투자신탁[채권혼합]ClassC-P</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1160,27 +1160,27 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2019-03-21</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2019-09-27</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve">             200</t>
+          <t xml:space="preserve">             375</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t xml:space="preserve">             206</t>
+          <t xml:space="preserve">             368</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>채권형</t>
+          <t>혼합채권형</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1190,27 +1190,27 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0.39</t>
+          <t>-1.98</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>1.40</t>
+          <t>-0.64</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-2.14</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2.89</t>
+          <t>3.90</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>0.14</t>
+          <t>0.89</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
@@ -1220,24 +1220,24 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>0.15</t>
+          <t>0.89</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.07</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>2-5</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>┖▷골든브릿지베스트증권투자신탁 1[채권]종류C-W</t>
+          <t>┖▷대신배당공모주알파30증권투자신탁[채권혼합]ClassC-P2</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -1248,27 +1248,27 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2019-03-21</t>
+          <t>2016-03-30</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2019-09-27</t>
+          <t>2016-03-28</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t xml:space="preserve">          54,455</t>
+          <t xml:space="preserve">              82</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t xml:space="preserve">          56,026</t>
+          <t xml:space="preserve">              80</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>채권형</t>
+          <t>혼합채권형</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1278,27 +1278,27 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0.39</t>
+          <t>-1.98</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>1.40</t>
+          <t>-0.64</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>-2.13</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>2.90</t>
+          <t>3.91</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>0.13</t>
+          <t>0.88</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1308,12 +1308,3972 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>0.14</t>
+          <t>0.88</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>대신공모주30증권모투자신탁[채권혼합]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2018-01-18</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2018-01-18</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           6,457</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           6,714</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>-0.19</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>1.45</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>3.85</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>6.95</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>대신인덱스밸류증권투자신탁[주식](운용)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2018-10-23</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2018-10-23</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          29,740</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          30,151</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>-5.75</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>5.52</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>-2.42</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>2.63</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>4-1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>┖▷대신인덱스밸류증권투자신탁[주식]ClassC-F</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2018-10-23</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2018-10-23</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          29,740</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          30,151</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>-5.76</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>5.40</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>-2.63</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>2.34</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>0.21</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>대신배당주증권자투자신탁 2[주식]</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2004-09-13</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             170</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             130</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>-6.80</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>-3.69</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>-13.17</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>53.75</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>대신배당주증권모투자신탁[주식]</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2006-02-21</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           4,900</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           3,827</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>-6.65</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>-2.94</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>-11.78</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>118.18</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>대신퇴직연금40 배당주증권자투자신탁 [채권혼합]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2006-02-21</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           4,035</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           3,895</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>-2.20</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>-1.13</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>-3.25</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>69.83</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>0.81</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>대신배당주증권자투자신탁 1[주식](운용)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2006-10-23</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             157</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             115</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>-6.51</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>-2.90</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>-11.50</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>47.44</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>8-1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 1[주식]Class A</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2006-10-23</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               3</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               2</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>-6.59</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>-3.31</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>-12.24</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>18.33</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>8-2</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 1[주식]Class C</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2006-10-23</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             151</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             110</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>-6.66</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>-3.64</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>-12.85</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>13.64</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>8-3</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 1[주식]Class C-e</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2006-10-23</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               4</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               3</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>-6.57</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>-3.20</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>-12.03</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>-1.62</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>대신배당주증권자투자신탁 6[주식](운용)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2007-10-01</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             188</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             141</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>-6.63</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>-2.93</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>-11.76</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>-4.42</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>9-2</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 6[주식]ClassA</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2007-10-01</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              88</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              68</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>-6.72</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>-3.36</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>-12.54</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>-14.05</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>9-3</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 6[주식]ClassC-e</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2007-10-01</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              15</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              11</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>-6.70</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>-3.25</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>-12.34</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>-13.88</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>9-4</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 6[주식]ClassC1</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2007-10-01</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              85</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              62</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>-6.78</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>-3.68</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>-13.13</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>-21.59</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>1.50</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>대신KOSPI200인덱스증권자투자신탁[주식-파생형](운용)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2002-01-07</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          30,872</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          32,708</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>115.83</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>10-1</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>┖▷대신KOSPI200인덱스증권자투자신탁[주식-파생형]ClassA</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2002-01-07</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          16,657</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          17,782</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>56.15</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>0.40</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>10-2</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>┖▷대신KOSPI200인덱스증권자투자신탁[주식-파생형]ClassA2</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2020-01-16</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             182</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             165</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>-5.67</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>-10.31</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>0.44</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>0.44</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>10-3</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>┖▷대신KOSPI200인덱스증권자투자신탁[주식-파생형]ClassAe</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2019-12-10</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           1,972</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           1,939</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>-5.66</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>-1.95</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>10-4</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>┖▷대신KOSPI200인덱스증권자투자신탁[주식-파생형]ClassC-P</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2016-09-05</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             360</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             396</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>-5.70</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>5.51</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>-3.02</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>15.73</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>10-5</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>┖▷대신KOSPI200인덱스증권자투자신탁[주식-파생형]ClassC-P1</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2014-05-16</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           2,046</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           2,263</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>-5.69</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>5.56</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>-2.91</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>18.75</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>10-6</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>┖▷대신KOSPI200인덱스증권자투자신탁[주식-파생형]ClassC-P1e</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2018-04-03</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             717</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             651</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>-5.67</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>5.41</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>-2.94</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>-10.08</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>10-7</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>┖▷대신KOSPI200인덱스증권자투자신탁[주식-파생형]ClassC-Pe</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2018-04-04</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           1,298</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           1,179</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>-5.67</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>5.38</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>-2.99</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>-9.99</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>10-9</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>┖▷대신KOSPI200인덱스증권자투자신탁[주식-파생형]ClassC-e</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2002-01-07</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           6,599</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           7,226</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>59.62</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>0.37</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>10-11</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>┖▷대신KOSPI200인덱스증권자투자신탁[주식-파생형]ClassC1</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2002-01-07</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2009-01-09</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           1,040</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           1,107</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>298.84</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>0.80</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>대신장기주택마련배당주증권자투자신탁 [주식](운용)</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2007-12-07</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              88</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              67</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>-6.54</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>-3.05</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>-11.33</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>3.94</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>11-1</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>┖▷대신장기주택마련배당주증권자투자신탁 [주식]Class A</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2007-12-07</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              88</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              67</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>-6.63</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>-3.57</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>-12.28</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>-10.39</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>1.05</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>1.05</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>대신연금저축배당주증권전환형자투자신탁[주식]</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2007-12-24</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           2,852</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           1,911</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>-6.75</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>-3.63</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>-13.03</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>-25.72</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>1.45</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>1.45</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>대신배당주증권자투자신탁 4[주식](운용)</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2008-01-03</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              48</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              36</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>-6.62</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>-2.90</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>-11.74</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>59.55</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>13-1</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 4[주식]Class A-e</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2008-01-03</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              33</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              25</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>-6.68</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>-3.22</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>-12.33</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>47.78</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>0.68</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>0.68</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>13-2</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 4[주식]Class C-e</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2008-01-03</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              15</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              12</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>-6.67</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>-3.21</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>-12.31</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>43.93</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>대신배당주증권자투자신탁 3[주식](운용)</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2008-09-05</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              11</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               8</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>-6.52</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>-3.13</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>-11.17</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>25.48</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>14-2</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 3[주식]Class A</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2008-09-05</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               0</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               0</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>-6.57</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>-3.45</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>-11.75</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>9.07</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>0.85</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>14-3</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>┖▷대신배당주증권자투자신탁 3[주식]ClassC-e</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2008-09-05</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              10</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               8</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>주식형</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>-6.57</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>-3.46</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>-11.75</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>17.22</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>0.65</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>대신밸런스배당주재형증권자투자신탁[채권혼합]</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2013-03-08</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2016-10-25</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              45</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              43</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>-0.91</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>1.19</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>-1.71</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>7.51</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>0.76</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>0.76</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>대신KOSPI200인덱스증권모투자신탁[주식-파생형]</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2013-05-16</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2013-05-16</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          28,763</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          32,269</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>-5.72</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>5.64</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>-2.36</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>29.17</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>대신소득공제장기KOSPI200인덱스증권자투자신탁[주식-파생형](운용)</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2014-03-19</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2014-03-19</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              11</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              13</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>-5.45</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>5.81</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>-1.98</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>29.77</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>17-1</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>┖▷대신소득공제장기KOSPI200인덱스증권자투자신탁[주식-파생형]ClassC</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2014-03-19</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>2014-03-19</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              10</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              11</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>-5.51</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>5.45</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>-2.73</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>24.18</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>0.70</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>17-2</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>┖▷대신소득공제장기KOSPI200인덱스증권자투자신탁[주식-파생형]ClassC-e</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2014-06-25</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>2014-03-19</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               1</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">               2</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>파생상품</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>-5.49</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>5.58</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>-2.45</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>22.43</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>0.45</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>대신공모주30증권자투자신탁 1[채권혼합](운용)</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2014-12-18</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>2014-12-18</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           5,881</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           6,136</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>-0.18</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>1.41</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>3.71</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>18.82</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>18-1</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>┖▷대신공모주30증권자투자신탁 1[채권혼합]ClassA</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2015-01-28</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>2014-12-18</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             723</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             757</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>-0.25</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>0.92</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>2.76</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>13.27</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>0.89</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>0.89</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>18-2</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>┖▷대신공모주30증권자투자신탁 1[채권혼합]ClassC</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2014-12-18</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>2014-12-18</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           5,076</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           5,298</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>-0.27</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>0.76</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>2.44</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>11.63</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>1.19</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>1.19</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>18-3</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>┖▷대신공모주30증권자투자신탁 1[채권혼합]ClassC-e</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2020-01-14</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>2014-12-18</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              82</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              81</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>-0.24</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>-0.26</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>0.79</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>0.79</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>대신공모주10증권투자신탁[채권혼합](운용)</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2014-12-15</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>2014-12-15</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           4,708</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           4,708</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>-0.01</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>0.96</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>2.57</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>17.63</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>19-1</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>┖▷대신공모주10증권투자신탁[채권혼합]Class C</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2014-12-15</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>2014-12-15</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           4,518</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           4,518</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>-0.10</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>0.36</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>1.37</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>10.59</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>1.19</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>1.19</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>19-2</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>┖▷대신공모주10증권투자신탁[채권혼합]ClassA</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>책임</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2016-01-19</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>2014-12-15</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             190</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">             190</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>혼합채권형</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>국내</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>-0.08</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>0.51</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>1.67</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>8.46</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>0.89</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>0.89</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>0.06</t>
         </is>
       </c>
     </row>

</xml_diff>